<commit_message>
Aggiunti al template gli altri due esercizi della verifica di GPOI: BEP e Analisi Investimenti.
</commit_message>
<xml_diff>
--- a/GPOI/Appunti/Template Esercizi Verifica.xlsx
+++ b/GPOI/Appunti/Template Esercizi Verifica.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scuola\Collegamento GitHub\GPOI\Appunti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC0CE98-F31E-461F-993A-A060AB28D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6B57C8-92D9-491A-9DBE-8221EC098BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{0087FA8B-F93B-45C6-8E70-570E54A69374}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{0087FA8B-F93B-45C6-8E70-570E54A69374}"/>
   </bookViews>
   <sheets>
-    <sheet name="Costi e Ricavi" sheetId="1" r:id="rId1"/>
+    <sheet name="BEP" sheetId="2" r:id="rId1"/>
+    <sheet name="Costi e Ricavi" sheetId="1" r:id="rId2"/>
+    <sheet name="Analisi Investimenti" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
   <si>
     <t>Studente</t>
   </si>
@@ -201,13 +203,114 @@
   </si>
   <si>
     <t>Quantità di massimo profitto</t>
+  </si>
+  <si>
+    <t>Cf tot</t>
+  </si>
+  <si>
+    <t>Costi fissi totali</t>
+  </si>
+  <si>
+    <t>Cvu</t>
+  </si>
+  <si>
+    <t>Costo variabile unitario</t>
+  </si>
+  <si>
+    <t>Pu</t>
+  </si>
+  <si>
+    <t>BEP</t>
+  </si>
+  <si>
+    <t>Break Even Point</t>
+  </si>
+  <si>
+    <t>Costi variabili</t>
+  </si>
+  <si>
+    <t>Cv</t>
+  </si>
+  <si>
+    <t>Ctot</t>
+  </si>
+  <si>
+    <t>Costo BEP</t>
+  </si>
+  <si>
+    <t>Costo corrispondente al BEP</t>
+  </si>
+  <si>
+    <t>Un'azienda vuole produrre siti web e investe inizialmente 50000 euro in infrastrutture e costi indiretti. Prevede un ricavo annuale di 20000 euro per almeno 3 anni e stabilisce un ROI del 25%. Calcolare la redditività della nuova produzione con i tre modi VAN, TIR e Payback.</t>
+  </si>
+  <si>
+    <t>Analisi Investimenti</t>
+  </si>
+  <si>
+    <t>Inv.</t>
+  </si>
+  <si>
+    <t>Investimento iniziale</t>
+  </si>
+  <si>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>Ricavo Annuale</t>
+  </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>Return on Investment</t>
+  </si>
+  <si>
+    <t>Anni</t>
+  </si>
+  <si>
+    <t>Movimenti</t>
+  </si>
+  <si>
+    <t>Tabella Movimenti</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>TIR</t>
+  </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>Calcolo per Payback Period</t>
+  </si>
+  <si>
+    <t>Payback Period</t>
+  </si>
+  <si>
+    <t>Valore Attuale Netto</t>
+  </si>
+  <si>
+    <t>Tasso Interno di Rendimento</t>
+  </si>
+  <si>
+    <t>Tasso di Recupero (in anni)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +354,20 @@
       <color theme="1"/>
       <name val="Cascadia Mono Light"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -429,19 +546,108 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -449,32 +655,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -485,36 +670,150 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="2" builtinId="5"/>
+    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
     <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF6161"/>
+          <bgColor rgb="FFFFA3A3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA3A3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -528,21 +827,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFA3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6161"/>
         </patternFill>
       </fill>
     </dxf>
@@ -556,7 +841,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFA3"/>
+          <bgColor rgb="FFFF6161"/>
         </patternFill>
       </fill>
     </dxf>
@@ -564,6 +849,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFA3A3"/>
+      <color rgb="FFFF7171"/>
       <color rgb="FF4188D7"/>
       <color rgb="FFFF6161"/>
       <color rgb="FFFFFFA3"/>
@@ -596,6 +883,755 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>BEP</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Costi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>BEP!$A$15:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>BEP!$D$15:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0\ "€"_-;\-* #,##0\ "€"_-;_-* "-"??\ "€"_-;_-@_-</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5F85-4558-83D2-7974A158DF9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ricavi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>BEP!$A$15:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>BEP!$E$15:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0\ "€"_-;\-* #,##0\ "€"_-;_-* "-"??\ "€"_-;_-@_-</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>48000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>51000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>54000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>57000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>60000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5F85-4558-83D2-7974A158DF9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BEP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>BEP!$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>BEP!$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0\ "€"_-;\-* #,##0\ "€"_-;_-* "-"??\ "€"_-;_-@_-</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5F85-4558-83D2-7974A158DF9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1781555327"/>
+        <c:axId val="1781559647"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1781555327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1781559647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1781559647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="60000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1781555327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Costi e Ricavi</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -654,7 +1690,7 @@
             <c:numRef>
               <c:f>'Costi e Ricavi'!$B$22:$B$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_("€"* #,##0.00_);_("€"* \(#,##0.00\);_("€"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -739,7 +1775,7 @@
             <c:numRef>
               <c:f>'Costi e Ricavi'!$C$22:$C$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_("€"* #,##0.00_);_("€"* \(#,##0.00\);_("€"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
@@ -806,7 +1842,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -867,7 +1903,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -916,6 +1952,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1000,6 +2067,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1516,20 +2623,577 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>352927</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>16043</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5494</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>364</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>190249</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>6769</xdr:rowOff>
+      <xdr:colOff>338869</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>91218</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{162311F0-8016-2E60-EFE7-A50F3314D1DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>808470</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>173412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>645792</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>44041</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1873,575 +3537,1291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885D9CC2-13BB-41C5-8316-27ED970CC12D}">
-  <dimension ref="A1:J28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D62AB7-6642-4E22-BD7A-613EF90EA581}">
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+      <c r="A1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="G1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="G3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="23">
+        <v>10000</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="35">
+        <v>45722</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="G4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="23">
+        <v>5</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="23">
+        <v>15</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+      <c r="A6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+      <c r="A7" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="G7" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="G9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="24">
+        <f>$H$3/($H$5-$H$4)</f>
+        <v>1000</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="G10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="23">
+        <f ca="1">OFFSET($E$14,MATCH($H$9,A15:A35,0),0)</f>
+        <v>15000</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+      <c r="A13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A15" s="16">
+        <v>0</v>
+      </c>
+      <c r="B15" s="25">
+        <f>$H$3</f>
+        <v>10000</v>
+      </c>
+      <c r="C15" s="25">
+        <f>A15*$H$4</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="25">
+        <f>B15+C15</f>
+        <v>10000</v>
+      </c>
+      <c r="E15" s="26">
+        <f>A15*$H$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A16" s="16">
+        <v>200</v>
+      </c>
+      <c r="B16" s="25">
+        <f t="shared" ref="B16:B35" si="0">$H$3</f>
+        <v>10000</v>
+      </c>
+      <c r="C16" s="25">
+        <f t="shared" ref="C16:C17" si="1">A16*$H$4</f>
+        <v>1000</v>
+      </c>
+      <c r="D16" s="25">
+        <f t="shared" ref="D16:D17" si="2">B16+C16</f>
+        <v>11000</v>
+      </c>
+      <c r="E16" s="26">
+        <f t="shared" ref="E16:E17" si="3">A16*$H$5</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A17" s="16">
+        <v>400</v>
+      </c>
+      <c r="B17" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C17" s="25">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="D17" s="25">
+        <f t="shared" si="2"/>
+        <v>12000</v>
+      </c>
+      <c r="E17" s="26">
+        <f t="shared" si="3"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A18" s="16">
+        <v>600</v>
+      </c>
+      <c r="B18" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C18" s="25">
+        <f t="shared" ref="C18:C35" si="4">A18*$H$4</f>
+        <v>3000</v>
+      </c>
+      <c r="D18" s="25">
+        <f t="shared" ref="D18:D35" si="5">B18+C18</f>
+        <v>13000</v>
+      </c>
+      <c r="E18" s="26">
+        <f t="shared" ref="E18:E35" si="6">A18*$H$5</f>
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A19" s="16">
+        <v>800</v>
+      </c>
+      <c r="B19" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C19" s="25">
+        <f t="shared" si="4"/>
+        <v>4000</v>
+      </c>
+      <c r="D19" s="25">
+        <f t="shared" si="5"/>
+        <v>14000</v>
+      </c>
+      <c r="E19" s="26">
+        <f t="shared" si="6"/>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A20" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B20" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C20" s="25">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="D20" s="25">
+        <f t="shared" si="5"/>
+        <v>15000</v>
+      </c>
+      <c r="E20" s="26">
+        <f t="shared" si="6"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A21" s="16">
+        <v>1200</v>
+      </c>
+      <c r="B21" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C21" s="25">
+        <f t="shared" si="4"/>
+        <v>6000</v>
+      </c>
+      <c r="D21" s="25">
+        <f t="shared" si="5"/>
+        <v>16000</v>
+      </c>
+      <c r="E21" s="26">
+        <f t="shared" si="6"/>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A22" s="16">
+        <v>1400</v>
+      </c>
+      <c r="B22" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C22" s="25">
+        <f t="shared" si="4"/>
+        <v>7000</v>
+      </c>
+      <c r="D22" s="25">
+        <f t="shared" si="5"/>
+        <v>17000</v>
+      </c>
+      <c r="E22" s="26">
+        <f t="shared" si="6"/>
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A23" s="16">
+        <v>1600</v>
+      </c>
+      <c r="B23" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C23" s="25">
+        <f t="shared" si="4"/>
+        <v>8000</v>
+      </c>
+      <c r="D23" s="25">
+        <f t="shared" si="5"/>
+        <v>18000</v>
+      </c>
+      <c r="E23" s="26">
+        <f t="shared" si="6"/>
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A24" s="16">
+        <v>1800</v>
+      </c>
+      <c r="B24" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C24" s="25">
+        <f t="shared" si="4"/>
+        <v>9000</v>
+      </c>
+      <c r="D24" s="25">
+        <f t="shared" si="5"/>
+        <v>19000</v>
+      </c>
+      <c r="E24" s="26">
+        <f t="shared" si="6"/>
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A25" s="16">
+        <v>2000</v>
+      </c>
+      <c r="B25" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C25" s="25">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="D25" s="25">
+        <f t="shared" si="5"/>
+        <v>20000</v>
+      </c>
+      <c r="E25" s="26">
+        <f t="shared" si="6"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A26" s="16">
+        <v>2200</v>
+      </c>
+      <c r="B26" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C26" s="25">
+        <f t="shared" si="4"/>
+        <v>11000</v>
+      </c>
+      <c r="D26" s="25">
+        <f t="shared" si="5"/>
+        <v>21000</v>
+      </c>
+      <c r="E26" s="26">
+        <f t="shared" si="6"/>
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A27" s="16">
+        <v>2400</v>
+      </c>
+      <c r="B27" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C27" s="25">
+        <f t="shared" si="4"/>
+        <v>12000</v>
+      </c>
+      <c r="D27" s="25">
+        <f t="shared" si="5"/>
+        <v>22000</v>
+      </c>
+      <c r="E27" s="26">
+        <f t="shared" si="6"/>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A28" s="16">
+        <v>2600</v>
+      </c>
+      <c r="B28" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C28" s="25">
+        <f t="shared" si="4"/>
+        <v>13000</v>
+      </c>
+      <c r="D28" s="25">
+        <f t="shared" si="5"/>
+        <v>23000</v>
+      </c>
+      <c r="E28" s="26">
+        <f t="shared" si="6"/>
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A29" s="16">
+        <v>2800</v>
+      </c>
+      <c r="B29" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C29" s="25">
+        <f t="shared" si="4"/>
+        <v>14000</v>
+      </c>
+      <c r="D29" s="25">
+        <f t="shared" si="5"/>
+        <v>24000</v>
+      </c>
+      <c r="E29" s="26">
+        <f t="shared" si="6"/>
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A30" s="16">
+        <v>3000</v>
+      </c>
+      <c r="B30" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C30" s="25">
+        <f t="shared" si="4"/>
+        <v>15000</v>
+      </c>
+      <c r="D30" s="25">
+        <f t="shared" si="5"/>
+        <v>25000</v>
+      </c>
+      <c r="E30" s="26">
+        <f t="shared" si="6"/>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A31" s="16">
+        <v>3200</v>
+      </c>
+      <c r="B31" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C31" s="25">
+        <f t="shared" si="4"/>
+        <v>16000</v>
+      </c>
+      <c r="D31" s="25">
+        <f t="shared" si="5"/>
+        <v>26000</v>
+      </c>
+      <c r="E31" s="26">
+        <f t="shared" si="6"/>
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A32" s="16">
+        <v>3400</v>
+      </c>
+      <c r="B32" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C32" s="25">
+        <f t="shared" si="4"/>
+        <v>17000</v>
+      </c>
+      <c r="D32" s="25">
+        <f t="shared" si="5"/>
+        <v>27000</v>
+      </c>
+      <c r="E32" s="26">
+        <f t="shared" si="6"/>
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A33" s="16">
+        <v>3600</v>
+      </c>
+      <c r="B33" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C33" s="25">
+        <f t="shared" si="4"/>
+        <v>18000</v>
+      </c>
+      <c r="D33" s="25">
+        <f t="shared" si="5"/>
+        <v>28000</v>
+      </c>
+      <c r="E33" s="26">
+        <f t="shared" si="6"/>
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A34" s="16">
+        <v>3800</v>
+      </c>
+      <c r="B34" s="25">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C34" s="25">
+        <f t="shared" si="4"/>
+        <v>19000</v>
+      </c>
+      <c r="D34" s="25">
+        <f t="shared" si="5"/>
+        <v>29000</v>
+      </c>
+      <c r="E34" s="26">
+        <f t="shared" si="6"/>
+        <v>57000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="19">
+        <v>4000</v>
+      </c>
+      <c r="B35" s="27">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C35" s="27">
+        <f t="shared" si="4"/>
+        <v>20000</v>
+      </c>
+      <c r="D35" s="27">
+        <f t="shared" si="5"/>
+        <v>30000</v>
+      </c>
+      <c r="E35" s="28">
+        <f t="shared" si="6"/>
+        <v>60000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A8:E11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885D9CC2-13BB-41C5-8316-27ED970CC12D}">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="10"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="G3" s="12" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="11"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="G4" s="12" t="s">
+      <c r="B4" s="35">
+        <v>45722</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="G4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="15">
         <v>30</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="29"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="15">
         <v>30</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="29"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="G6" s="12" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="G6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="15">
         <v>32</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="11"/>
+      <c r="J6" s="29"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="G7" s="12" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="G7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="15">
         <v>35</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="29"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="G8" s="12" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="G8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="15">
         <v>43</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="29"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="G9" s="12" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="G9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="15">
         <v>58</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="11"/>
+      <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="G10" s="12" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="G10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="15">
         <v>120</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="11"/>
+      <c r="J10" s="29"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="30"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="15">
         <v>15</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="29"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="15">
         <v>30</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16" s="29"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="15">
         <f>MAX(H22:H28)</f>
         <v>17</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="29"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="5">
         <f ca="1">OFFSET(A21,MATCH($B$17,H22:H28,0),0)</f>
         <v>4</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.45">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
-      <c r="A22" s="20">
+      <c r="A22" s="16">
         <v>0</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="17">
         <f>A22*$B$15</f>
         <v>0</v>
       </c>
-      <c r="C22" s="13">
-        <f>H4</f>
+      <c r="C22" s="17">
+        <f t="shared" ref="C22:C28" si="0">H4</f>
         <v>30</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="13" t="str">
+      <c r="G22" s="7" t="str">
         <f>IF(F22&gt;0, "Aumentare", IF(F22&lt;0, "Diminuire", "Mantieni"))</f>
         <v>Aumentare</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H22" s="18">
         <f>B22-C22</f>
         <v>-30</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
-      <c r="A23" s="20">
+      <c r="A23" s="16">
         <v>1</v>
       </c>
-      <c r="B23" s="13">
-        <f t="shared" ref="B23:B28" si="0">A23*$B$15</f>
+      <c r="B23" s="17">
+        <f t="shared" ref="B23:B28" si="1">A23*$B$15</f>
         <v>15</v>
       </c>
-      <c r="C23" s="13">
-        <f>H5</f>
+      <c r="C23" s="17">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="17">
         <f>B23-B22</f>
         <v>15</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="17">
         <f>C23-C22</f>
         <v>0</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="17">
         <f>D23-E23</f>
         <v>15</v>
       </c>
-      <c r="G23" s="13" t="str">
-        <f t="shared" ref="G23:G28" si="1">IF(F23&gt;0, "Aumentare", IF(F23&lt;0, "Diminuire", "Mantieni"))</f>
+      <c r="G23" s="7" t="str">
+        <f t="shared" ref="G23:G28" si="2">IF(F23&gt;0, "Aumentare", IF(F23&lt;0, "Diminuire", "Mantieni"))</f>
         <v>Aumentare</v>
       </c>
-      <c r="H23" s="21">
-        <f t="shared" ref="H23:H28" si="2">B23-C23</f>
+      <c r="H23" s="18">
+        <f t="shared" ref="H23:H28" si="3">B23-C23</f>
         <v>-15</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
-      <c r="A24" s="20">
+      <c r="A24" s="16">
         <v>2</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="17">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C24" s="17">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="C24" s="13">
-        <f>H6</f>
         <v>32</v>
       </c>
-      <c r="D24" s="13">
-        <f t="shared" ref="D24:E28" si="3">B24-B23</f>
+      <c r="D24" s="17">
+        <f t="shared" ref="D24:E28" si="4">B24-B23</f>
         <v>15</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F24" s="17">
+        <f t="shared" ref="F24:F28" si="5">D24-E24</f>
+        <v>13</v>
+      </c>
+      <c r="G24" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Aumentare</v>
+      </c>
+      <c r="H24" s="18">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="F24" s="13">
-        <f t="shared" ref="F24:F28" si="4">D24-E24</f>
-        <v>13</v>
-      </c>
-      <c r="G24" s="13" t="str">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A25" s="16">
+        <v>3</v>
+      </c>
+      <c r="B25" s="17">
         <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="C25" s="17">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D25" s="17">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="E25" s="17">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F25" s="17">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G25" s="7" t="str">
+        <f t="shared" si="2"/>
         <v>Aumentare</v>
       </c>
-      <c r="H24" s="21">
+      <c r="H25" s="18">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A26" s="16">
+        <v>4</v>
+      </c>
+      <c r="B26" s="17">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="C26" s="17">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D26" s="17">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="E26" s="17">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="F26" s="17">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
-      <c r="A25" s="20">
-        <v>3</v>
-      </c>
-      <c r="B25" s="13">
+        <v>Aumentare</v>
+      </c>
+      <c r="H26" s="18">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
+      <c r="A27" s="16">
+        <v>5</v>
+      </c>
+      <c r="B27" s="17">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="C27" s="17">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="C25" s="13">
-        <f>H7</f>
-        <v>35</v>
-      </c>
-      <c r="D25" s="13">
+        <v>58</v>
+      </c>
+      <c r="D27" s="17">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="E27" s="17">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="F27" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Mantieni</v>
+      </c>
+      <c r="H27" s="18">
         <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="19">
+        <v>6</v>
+      </c>
+      <c r="B28" s="20">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="C28" s="20">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="D28" s="20">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E28" s="20">
+        <f t="shared" si="4"/>
+        <v>62</v>
+      </c>
+      <c r="F28" s="20">
+        <f t="shared" si="5"/>
+        <v>-47</v>
+      </c>
+      <c r="G28" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>Diminuire</v>
+      </c>
+      <c r="H28" s="21">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="F25" s="13">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="G25" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Aumentare</v>
-      </c>
-      <c r="H25" s="21">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
-      <c r="A26" s="20">
-        <v>4</v>
-      </c>
-      <c r="B26" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="C26" s="13">
-        <f>H8</f>
-        <v>43</v>
-      </c>
-      <c r="D26" s="13">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="E26" s="13">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="F26" s="13">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="G26" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Aumentare</v>
-      </c>
-      <c r="H26" s="21">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16.149999999999999" x14ac:dyDescent="0.45">
-      <c r="A27" s="20">
-        <v>5</v>
-      </c>
-      <c r="B27" s="13">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="C27" s="13">
-        <f>H9</f>
-        <v>58</v>
-      </c>
-      <c r="D27" s="13">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="E27" s="13">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="F27" s="13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Mantieni</v>
-      </c>
-      <c r="H27" s="21">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="22">
-        <v>6</v>
-      </c>
-      <c r="B28" s="23">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="C28" s="23">
-        <f>H10</f>
-        <v>120</v>
-      </c>
-      <c r="D28" s="23">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="E28" s="23">
-        <f t="shared" si="3"/>
-        <v>62</v>
-      </c>
-      <c r="F28" s="23">
-        <f t="shared" si="4"/>
-        <v>-47</v>
-      </c>
-      <c r="G28" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>Diminuire</v>
-      </c>
-      <c r="H28" s="24">
-        <f t="shared" si="2"/>
         <v>-30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B2:E2"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="A8:E11"/>
     <mergeCell ref="G1:J1"/>
@@ -2457,22 +4837,23 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="G22:G28">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Diminuire"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Mantieni"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Aumentare"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>"Mantieni"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
-      <formula>"Diminuire"</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H28">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2481,11 +4862,374 @@
         <color theme="6" tint="0.59999389629810485"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EABF4EF-50E1-4977-BD6E-E67B7E93A7F8}">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+      <c r="A1" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+      <c r="G1" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="41"/>
+      <c r="G2" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="64"/>
+      <c r="K2" s="70"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="41"/>
+      <c r="G3" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="65">
+        <v>-50000</v>
+      </c>
+      <c r="I3" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="66"/>
+      <c r="K3" s="72"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="43">
+        <v>45722</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
+      <c r="G4" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="65">
+        <v>20000</v>
+      </c>
+      <c r="I4" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="66"/>
+      <c r="K4" s="72"/>
+    </row>
+    <row r="5" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="67">
+        <v>3</v>
+      </c>
+      <c r="I5" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="66"/>
+      <c r="K5" s="72"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+      <c r="G6" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="75">
+        <v>0.25</v>
+      </c>
+      <c r="I6" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" s="76"/>
+      <c r="K6" s="77"/>
+    </row>
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="49"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+      <c r="A8" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="51"/>
+      <c r="G8" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="39"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="50"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="51"/>
+      <c r="G9" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="64"/>
+      <c r="K9" s="70"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="50"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="51"/>
+      <c r="G10" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="78">
+        <f>NPV(H6,C15:E15)+$B$15</f>
+        <v>-10960</v>
+      </c>
+      <c r="I10" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="66"/>
+      <c r="K10" s="72"/>
+    </row>
+    <row r="11" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="52"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
+      <c r="G11" s="73" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="68">
+        <f>IRR(B15:E15)</f>
+        <v>9.7010257403348898E-2</v>
+      </c>
+      <c r="I11" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="66"/>
+      <c r="K11" s="72"/>
+    </row>
+    <row r="12" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G12" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="79">
+        <f>SUM(B17:E17)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I12" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="76"/>
+      <c r="K12" s="77"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="55">
+        <v>0</v>
+      </c>
+      <c r="C14" s="55">
+        <v>1</v>
+      </c>
+      <c r="D14" s="55">
+        <v>2</v>
+      </c>
+      <c r="E14" s="58">
+        <v>3</v>
+      </c>
+      <c r="G14" s="80" t="str">
+        <f>IF(H10&lt;0,"VAN negativo","")</f>
+        <v>VAN negativo</v>
+      </c>
+      <c r="H14" s="81" t="str">
+        <f>IF(G14="VAN negativo","Redditività negativa!","")</f>
+        <v>Redditività negativa!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="56">
+        <f>$H$3</f>
+        <v>-50000</v>
+      </c>
+      <c r="C15" s="56">
+        <f>$H$4</f>
+        <v>20000</v>
+      </c>
+      <c r="D15" s="56">
+        <f t="shared" ref="D15:E15" si="0">$H$4</f>
+        <v>20000</v>
+      </c>
+      <c r="E15" s="59">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="G15" s="82" t="str">
+        <f>IF(H11&lt;H6,"TIR &lt; ROI","")</f>
+        <v>TIR &lt; ROI</v>
+      </c>
+      <c r="H15" s="83" t="str">
+        <f>IF(G15="TIR &lt; ROI","Redditività negativa!","")</f>
+        <v>Redditività negativa!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="56">
+        <f>$H$3</f>
+        <v>-50000</v>
+      </c>
+      <c r="C16" s="56">
+        <f>B16+C15</f>
+        <v>-30000</v>
+      </c>
+      <c r="D16" s="56">
+        <f t="shared" ref="D16:E16" si="1">C16+D15</f>
+        <v>-10000</v>
+      </c>
+      <c r="E16" s="59">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="61">
+        <f>IF(AND(B16&lt;0,B15&gt;0),1,IF(B16&lt;B15,B16/B15,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="61">
+        <f t="shared" ref="C17:E17" si="2">IF(AND(C16&lt;0,C15&gt;0),1,IF(C16&lt;C15,C16/C15,0))</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="61">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="62">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A8:E11"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="I3:K3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G14:H15">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(G14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>